<commit_message>
excel sheet with formulas
</commit_message>
<xml_diff>
--- a/camToRobot.xlsx
+++ b/camToRobot.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RaminMohammadi_REU2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6031B930-3179-479F-B696-BA63A91A735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC5CEEE4-4FBB-4D29-B607-84EDDB5D4516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA580C8B-B8DD-470E-BC58-A8F88DB302D1}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{EA580C8B-B8DD-470E-BC58-A8F88DB302D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>robot x-</t>
   </si>
@@ -124,6 +125,27 @@
   </si>
   <si>
     <t>TEST FORMULA Linear x+</t>
+  </si>
+  <si>
+    <t>New x+ DATA</t>
+  </si>
+  <si>
+    <t>cam+_x(px)</t>
+  </si>
+  <si>
+    <t>robot+xmm</t>
+  </si>
+  <si>
+    <t>X+  outlier</t>
+  </si>
+  <si>
+    <t>TEST FORMULA QUADRATIC, new x+</t>
+  </si>
+  <si>
+    <t>TEST FORMULA LINEAR, new x+</t>
+  </si>
+  <si>
+    <t>QUADRATIC Y+ BAD</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1417,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11506209127145486"/>
+          <c:y val="8.9854391600676625E-2"/>
+          <c:w val="0.77048908719553399"/>
+          <c:h val="0.61688691565359655"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1428,7 +1460,10 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -1436,13 +1471,15 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
+            <c:forward val="500"/>
+            <c:backward val="150"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.49281671041119862"/>
-                  <c:y val="-0.56773877223680369"/>
+                  <c:x val="-8.9568686377219334E-2"/>
+                  <c:y val="0.27161306341957536"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1486,13 +1523,15 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="500"/>
+            <c:backward val="150"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.5854768153980753E-2"/>
-                  <c:y val="0.35673264800233306"/>
+                  <c:x val="-9.3290599272601818E-2"/>
+                  <c:y val="0.29017233830733458"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1649,6 +1688,7 @@
         <c:axId val="606334448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1080"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1893,6 +1933,791 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76180773202759977"/>
+          <c:y val="0.79483314264055194"/>
+          <c:w val="0.19801252648815737"/>
+          <c:h val="0.15117681664853791"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>New x+</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1346955778254991"/>
+          <c:y val="8.5365473473931169E-2"/>
+          <c:w val="0.82371232005090278"/>
+          <c:h val="0.58921103951397269"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:forward val="1000"/>
+            <c:backward val="600"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.20365069750896522"/>
+                  <c:y val="0.65946809688000774"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="1000"/>
+            <c:backward val="600"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.19484737484737485"/>
+                  <c:y val="0.78623385969105819"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="100"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$58:$S$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>851</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1067</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1157</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1185</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1314</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1414</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$58:$T$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>56.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>153.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>189.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>227.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>287.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>311.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>342.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>376.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>394.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>485.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>567.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>606.29999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B34-4570-9207-43578BCFFCC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="810118991"/>
+        <c:axId val="810119471"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="810118991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1920"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>cam x+</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46424139290281025"/>
+              <c:y val="0.70748385779598844"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="810119471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="810119471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>robot x+</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5477153911554449E-2"/>
+              <c:y val="0.39068590804312436"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="810118991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81332929537653942"/>
+          <c:y val="0.7604634380405686"/>
+          <c:w val="0.16047551748339151"/>
+          <c:h val="0.23953656195943135"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2057,6 +2882,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3090,6 +3955,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3682,15 +5063,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>280986</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3715,7 +5096,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42D87F17-1100-886C-329F-F38582873C96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4035,10 +5456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED33413A-F47E-493A-B34B-4E731ACFC891}">
-  <dimension ref="A1:V95"/>
+  <dimension ref="A1:Y96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="O86" sqref="O86"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O77" sqref="O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4245,18 +5666,18 @@
         <v>524.30399999999997</v>
       </c>
       <c r="O37">
-        <v>2</v>
+        <v>717</v>
       </c>
       <c r="P37" cm="1">
         <f t="array" ref="P37:P46">-0.00006 * O37:O46 ^2 + 0.8721 * O37:O46 -538.21</f>
-        <v>-536.46604000000002</v>
+        <v>56.24036000000001</v>
       </c>
       <c r="S37">
-        <v>2</v>
+        <v>717</v>
       </c>
       <c r="T37" cm="1">
         <f t="array" ref="T37:T46">0.7477 * S37:S46 -477.32</f>
-        <v>-475.82459999999998</v>
+        <v>58.780900000000031</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -4437,22 +5858,27 @@
         <v>525.38</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>525.38</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>525.38</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -4460,129 +5886,262 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>152</v>
       </c>
       <c r="B57">
         <v>466.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S57" t="s">
+        <v>23</v>
+      </c>
+      <c r="T57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>175</v>
       </c>
       <c r="B58">
         <v>449.6</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S58">
+        <v>718</v>
+      </c>
+      <c r="T58">
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>196</v>
       </c>
       <c r="B59">
         <v>433.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S59">
+        <v>684</v>
+      </c>
+      <c r="T59">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>218</v>
       </c>
       <c r="B60">
         <v>416.9</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S60">
+        <v>800</v>
+      </c>
+      <c r="T60">
+        <v>118.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>243</v>
       </c>
       <c r="B61">
         <v>369.9</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S61">
+        <v>824</v>
+      </c>
+      <c r="T61">
+        <v>132.69999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>265</v>
       </c>
       <c r="B62">
         <v>378.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S62">
+        <v>851</v>
+      </c>
+      <c r="T62">
+        <v>153.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>298.5</v>
       </c>
       <c r="B63">
         <v>356.2</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="S63">
+        <v>901</v>
+      </c>
+      <c r="T63">
+        <v>189.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>339.5</v>
       </c>
       <c r="B64">
         <v>325.7</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S64">
+        <v>951</v>
+      </c>
+      <c r="T64">
+        <v>227.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>371</v>
       </c>
       <c r="B65">
         <v>305.2</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O65" t="s">
+        <v>25</v>
+      </c>
+      <c r="P65">
+        <v>993</v>
+      </c>
+      <c r="Q65">
+        <v>356</v>
+      </c>
+      <c r="S65">
+        <v>993</v>
+      </c>
+      <c r="T65">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>405</v>
       </c>
       <c r="B66">
         <v>278.7</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S66">
+        <v>1038</v>
+      </c>
+      <c r="T66">
+        <v>287.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>446</v>
       </c>
       <c r="B67">
         <v>249.3</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S67">
+        <v>1067</v>
+      </c>
+      <c r="T67">
+        <v>311.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>473</v>
       </c>
       <c r="B68">
         <v>229.3</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S68">
+        <v>1110</v>
+      </c>
+      <c r="T68">
+        <v>342.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>505</v>
       </c>
       <c r="B69">
         <v>206</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S69">
+        <v>1157</v>
+      </c>
+      <c r="T69">
+        <v>376.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>544</v>
       </c>
       <c r="B70">
         <v>177.9</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="S70">
+        <v>1185</v>
+      </c>
+      <c r="T70">
+        <v>394.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S71">
+        <v>1275</v>
+      </c>
+      <c r="T71">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S72">
+        <v>1314</v>
+      </c>
+      <c r="T72">
+        <v>485.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S73">
+        <v>1414</v>
+      </c>
+      <c r="T73">
+        <v>567.79999999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S74">
+        <v>1468</v>
+      </c>
+      <c r="T74">
+        <v>606.29999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>28</v>
+      </c>
+      <c r="O78" s="1">
+        <v>-9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -4590,7 +6149,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S80" t="s">
+        <v>26</v>
+      </c>
+      <c r="X80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -4604,107 +6171,193 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>2</v>
+        <v>405</v>
       </c>
       <c r="B82" cm="1">
         <f t="array" ref="B82:B95">-0.0001*A82:A95^2 - 0.8133 * A82:A95 + 584.43</f>
-        <v>582.803</v>
+        <v>238.64099999999996</v>
       </c>
       <c r="F82">
-        <v>2</v>
+        <v>405</v>
       </c>
       <c r="G82" cm="1">
         <f t="array" ref="G82:G95">-0.7238*F82:F95 + 571.1</f>
-        <v>569.65240000000006</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <v>277.96100000000001</v>
+      </c>
+      <c r="S82" t="s">
+        <v>15</v>
+      </c>
+      <c r="T82" t="s">
+        <v>16</v>
+      </c>
+      <c r="X82" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>3</v>
+        <v>262</v>
       </c>
       <c r="B83">
-        <v>581.98919999999998</v>
+        <v>364.48099999999999</v>
       </c>
       <c r="F83">
-        <v>3</v>
+        <v>262</v>
       </c>
       <c r="G83">
-        <v>568.92860000000007</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <v>381.46440000000001</v>
+      </c>
+      <c r="S83">
+        <v>695</v>
+      </c>
+      <c r="T83" cm="1">
+        <f t="array" ref="T83:T96">-0.00009*S83:S96^2 + 0.9203 * S83:S96 - 556.75</f>
+        <v>39.386250000000018</v>
+      </c>
+      <c r="X83">
+        <v>695</v>
+      </c>
+      <c r="Y83" cm="1">
+        <f t="array" ref="Y83:Y96">0.7249*X83:X96 -457.09</f>
+        <v>46.71550000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="B84">
-        <v>581.1751999999999</v>
+        <v>472.81199999999995</v>
       </c>
       <c r="F84">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="G84">
-        <v>568.20479999999998</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <v>473.38700000000006</v>
+      </c>
+      <c r="S84">
+        <v>847</v>
+      </c>
+      <c r="T84">
+        <v>158.17728999999997</v>
+      </c>
+      <c r="X84">
+        <v>847</v>
+      </c>
+      <c r="Y84">
+        <v>156.90029999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>669</v>
+        <v>451</v>
       </c>
       <c r="B85">
-        <v>-4.4238000000001421</v>
+        <v>197.29159999999996</v>
       </c>
       <c r="F85">
-        <v>669</v>
+        <v>451</v>
       </c>
       <c r="G85">
-        <v>86.877800000000036</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <v>244.6662</v>
+      </c>
+      <c r="S85">
+        <v>940</v>
+      </c>
+      <c r="T85">
+        <v>228.80799999999999</v>
+      </c>
+      <c r="X85">
+        <v>940</v>
+      </c>
+      <c r="Y85">
+        <v>224.31599999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>300</v>
+        <v>483</v>
       </c>
       <c r="B86">
-        <v>331.43999999999994</v>
+        <v>168.27719999999994</v>
       </c>
       <c r="F86">
-        <v>300</v>
+        <v>483</v>
       </c>
       <c r="G86">
-        <v>353.96000000000004</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <v>221.50460000000004</v>
+      </c>
+      <c r="S86">
+        <v>1133</v>
+      </c>
+      <c r="T86">
+        <v>370.41789000000006</v>
+      </c>
+      <c r="X86">
+        <v>1133</v>
+      </c>
+      <c r="Y86">
+        <v>364.2217</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87">
+        <v>680</v>
+      </c>
+      <c r="B87">
+        <v>-14.854000000000042</v>
+      </c>
+      <c r="F87">
+        <v>680</v>
+      </c>
+      <c r="G87">
+        <v>78.915999999999997</v>
+      </c>
+      <c r="S87">
+        <v>1462</v>
+      </c>
+      <c r="T87">
+        <v>596.35863999999992</v>
+      </c>
+      <c r="X87">
+        <v>1462</v>
+      </c>
+      <c r="Y87">
+        <v>602.71379999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>468</v>
+      </c>
+      <c r="B88">
+        <v>181.90319999999991</v>
+      </c>
+      <c r="F88">
+        <v>468</v>
+      </c>
+      <c r="G88">
+        <v>232.36160000000001</v>
+      </c>
+      <c r="S88">
         <v>463</v>
       </c>
-      <c r="B87">
-        <v>186.43519999999995</v>
-      </c>
-      <c r="F87">
+      <c r="T88">
+        <v>-149.94430999999997</v>
+      </c>
+      <c r="X88">
         <v>463</v>
       </c>
-      <c r="G87">
-        <v>235.98060000000004</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>300</v>
-      </c>
-      <c r="B88">
-        <v>331.43999999999994</v>
-      </c>
-      <c r="F88">
-        <v>300</v>
-      </c>
-      <c r="G88">
-        <v>353.96000000000004</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Y88">
+        <v>-121.46129999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>561.5</v>
       </c>
@@ -4712,13 +6365,25 @@
         <v>96.233824999999911</v>
       </c>
       <c r="F89">
-        <v>561.5</v>
+        <v>336</v>
       </c>
       <c r="G89">
-        <v>164.68630000000002</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>327.90320000000003</v>
+      </c>
+      <c r="S89">
+        <v>709</v>
+      </c>
+      <c r="T89">
+        <v>50.501409999999964</v>
+      </c>
+      <c r="X89">
+        <v>709</v>
+      </c>
+      <c r="Y89">
+        <v>56.864100000000064</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>653</v>
       </c>
@@ -4731,8 +6396,20 @@
       <c r="G90">
         <v>98.458600000000047</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="S90">
+        <v>683</v>
+      </c>
+      <c r="T90">
+        <v>29.830889999999954</v>
+      </c>
+      <c r="X90">
+        <v>683</v>
+      </c>
+      <c r="Y90">
+        <v>38.016700000000014</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>318.5</v>
       </c>
@@ -4740,16 +6417,28 @@
         <v>315.24972499999996</v>
       </c>
       <c r="F91">
-        <v>318.5</v>
+        <v>210</v>
       </c>
       <c r="G91">
-        <v>340.56970000000001</v>
+        <v>419.10200000000003</v>
       </c>
       <c r="I91" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="S91">
+        <v>709</v>
+      </c>
+      <c r="T91">
+        <v>50.501409999999964</v>
+      </c>
+      <c r="X91">
+        <v>709</v>
+      </c>
+      <c r="Y91">
+        <v>56.864100000000064</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>554</v>
       </c>
@@ -4762,16 +6451,46 @@
       <c r="G92">
         <v>170.1148</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="S92">
+        <v>318.5</v>
+      </c>
+      <c r="T92">
+        <v>-272.7642525</v>
+      </c>
+      <c r="X92">
+        <v>318.5</v>
+      </c>
+      <c r="Y92">
+        <v>-226.20934999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>347</v>
+      </c>
       <c r="B93">
-        <v>584.42999999999995</v>
+        <v>290.17399999999992</v>
+      </c>
+      <c r="F93">
+        <v>347</v>
       </c>
       <c r="G93">
-        <v>571.1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>319.94140000000004</v>
+      </c>
+      <c r="S93">
+        <v>554</v>
+      </c>
+      <c r="T93">
+        <v>-74.526239999999973</v>
+      </c>
+      <c r="X93">
+        <v>554</v>
+      </c>
+      <c r="Y93">
+        <v>-55.495399999999961</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>144</v>
       </c>
@@ -4784,8 +6503,20 @@
       <c r="G94">
         <v>466.87280000000004</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="S94">
+        <v>347</v>
+      </c>
+      <c r="T94">
+        <v>-248.24270999999999</v>
+      </c>
+      <c r="X94">
+        <v>347</v>
+      </c>
+      <c r="Y94">
+        <v>-205.54969999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>528</v>
       </c>
@@ -4797,6 +6528,32 @@
       </c>
       <c r="G95">
         <v>188.93360000000001</v>
+      </c>
+      <c r="S95">
+        <v>144</v>
+      </c>
+      <c r="T95">
+        <v>-426.09303999999997</v>
+      </c>
+      <c r="X95">
+        <v>144</v>
+      </c>
+      <c r="Y95">
+        <v>-352.70439999999996</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S96">
+        <v>528</v>
+      </c>
+      <c r="T96">
+        <v>-95.922159999999963</v>
+      </c>
+      <c r="X96">
+        <v>528</v>
+      </c>
+      <c r="Y96">
+        <v>-74.342799999999954</v>
       </c>
     </row>
   </sheetData>
@@ -5082,16 +6839,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EE8125B-E63F-4851-830E-D1E1608D4F20}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d572115d-02d2-4f67-9461-466620dcdeda"/>
+    <ds:schemaRef ds:uri="0515279f-12bd-4590-9996-adf514ac7d06"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d572115d-02d2-4f67-9461-466620dcdeda"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0515279f-12bd-4590-9996-adf514ac7d06"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>